<commit_message>
Added defects in failed test cases
</commit_message>
<xml_diff>
--- a/Docs/08-Prueba/Tests Cases - Modulo de Agenda de Actividades.xlsx
+++ b/Docs/08-Prueba/Tests Cases - Modulo de Agenda de Actividades.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18675" windowHeight="8220" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="405" windowWidth="18675" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="US_93" sheetId="3" r:id="rId1"/>
-    <sheet name="US_87" sheetId="29" r:id="rId2"/>
-    <sheet name="Reference" sheetId="27" r:id="rId3"/>
+    <sheet name="Reference" sheetId="27" r:id="rId1"/>
+    <sheet name="US_93" sheetId="3" r:id="rId2"/>
+    <sheet name="US_87" sheetId="29" r:id="rId3"/>
     <sheet name="US_88" sheetId="30" r:id="rId4"/>
     <sheet name="US_89" sheetId="31" r:id="rId5"/>
     <sheet name="US_97" sheetId="32" r:id="rId6"/>
     <sheet name="US_99" sheetId="33" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">US_87!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">US_87!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="156">
   <si>
     <t>Application</t>
   </si>
@@ -473,6 +473,24 @@
   </si>
   <si>
     <t xml:space="preserve">Seleccionar la opción "Editar" en la reunión programada para el 23/05. </t>
+  </si>
+  <si>
+    <t>17/18</t>
+  </si>
+  <si>
+    <t>TC7_US93</t>
+  </si>
+  <si>
+    <t>Valida que al ingresar una descripción muy extensa, esta no se muestre en una sola línea en el  listado de eventos de agenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario ingresa una descripción sobre los contenidos que se tomarán en dicha evaluación lo suficientemente extensa (100 o 150 caracteres). </t>
+  </si>
+  <si>
+    <t>El sistema notifica que los cambios se han guardado exitosamente (el nuevo evento aparece en la agenda en forma multilinea de ser necesario).</t>
+  </si>
+  <si>
+    <t>Por el momento no se está grabando de ese modo.</t>
   </si>
 </sst>
 </file>
@@ -983,10 +1001,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1643,7 +1703,9 @@
       <c r="I35" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J35" s="6"/>
+      <c r="J35" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="42.75" thickBot="1">
       <c r="A36" s="7"/>
@@ -2189,8 +2251,212 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
+    <row r="67" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A67" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" s="3">
+        <v>1</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G67" s="4"/>
+      <c r="H67" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A68" s="7"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="3">
+        <v>2</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+    </row>
+    <row r="69" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A69" s="7"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="3">
+        <v>3</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A70" s="7"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="3">
+        <v>4</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G70" s="4"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+    </row>
+    <row r="71" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A71" s="7"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="3">
+        <v>5</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" s="4"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A72" s="7"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="3">
+        <v>6</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A73" s="7"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="3">
+        <v>7</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" ht="53.25" thickBot="1">
+      <c r="A74" s="7"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="3">
+        <v>8</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A75" s="7"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="3">
+        <v>9</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G75" s="4"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="1:10" ht="53.25" thickBot="1">
+      <c r="A76" s="7"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="3">
+        <v>10</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H76" s="15"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="42">
+    <mergeCell ref="J67:J76"/>
+    <mergeCell ref="A67:A76"/>
+    <mergeCell ref="B67:B76"/>
+    <mergeCell ref="C67:C76"/>
+    <mergeCell ref="H67:H76"/>
+    <mergeCell ref="I67:I76"/>
     <mergeCell ref="J35:J44"/>
     <mergeCell ref="A46:A55"/>
     <mergeCell ref="B46:B55"/>
@@ -2237,13 +2503,13 @@
           <x14:formula1>
             <xm:f>Reference!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H11 H13:H22 H24:H33 H35:H44 H46:H55 H57:H65</xm:sqref>
+          <xm:sqref>H2:H11 H13:H22 H24:H33 H35:H44 H46:H55 H57:H65 H67:H76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$C$1:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I11 I13:I22 I24:I33 I35:I44 I46:I55 I57:I65</xm:sqref>
+          <xm:sqref>I2:I11 I13:I22 I24:I33 I35:I44 I46:I55 I57:I65 I67:I76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2251,12 +2517,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A31" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2325,7 +2591,9 @@
       <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6"/>
+      <c r="J2" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="42.75" thickBot="1">
       <c r="A3" s="7"/>
@@ -2499,8 +2767,8 @@
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="14" t="s">
-        <v>16</v>
+      <c r="H12" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>11</v>
@@ -2521,7 +2789,7 @@
         <v>23</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="15"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
@@ -2539,7 +2807,7 @@
         <v>26</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
@@ -2559,7 +2827,7 @@
       <c r="G15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
     </row>
@@ -2575,7 +2843,7 @@
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
@@ -2591,7 +2859,7 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="15"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
     </row>
@@ -2607,7 +2875,7 @@
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="15"/>
+      <c r="H18" s="13"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
@@ -2625,7 +2893,7 @@
         <v>34</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="15"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
@@ -2643,7 +2911,7 @@
         <v>120</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="15"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
@@ -2679,13 +2947,15 @@
         <v>24</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="14" t="s">
-        <v>16</v>
+      <c r="H22" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="J22" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="42.75" thickBot="1">
       <c r="A23" s="7"/>
@@ -2701,7 +2971,7 @@
         <v>23</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="15"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
@@ -2719,7 +2989,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
@@ -2739,7 +3009,7 @@
       <c r="G25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
@@ -2755,7 +3025,7 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="15"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
@@ -2771,7 +3041,7 @@
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="15"/>
+      <c r="H27" s="13"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
@@ -2789,7 +3059,7 @@
         <v>34</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="15"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
@@ -2807,7 +3077,7 @@
         <v>51</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="15"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
@@ -2843,13 +3113,15 @@
         <v>24</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="14" t="s">
-        <v>16</v>
+      <c r="H31" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="6"/>
+      <c r="J31" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:10" ht="42.75" thickBot="1">
       <c r="A32" s="7"/>
@@ -2865,7 +3137,7 @@
         <v>23</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="15"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
     </row>
@@ -2883,7 +3155,7 @@
         <v>26</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="15"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
     </row>
@@ -2903,7 +3175,7 @@
       <c r="G34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="15"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
     </row>
@@ -2919,7 +3191,7 @@
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="15"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
@@ -2935,7 +3207,7 @@
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="15"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
     </row>
@@ -2953,7 +3225,7 @@
         <v>34</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="15"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
@@ -2973,7 +3245,7 @@
       <c r="G38" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H38" s="15"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
@@ -3190,53 +3462,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99:C109"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4137,7 +4368,9 @@
       <c r="I50" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J50" s="6"/>
+      <c r="J50" s="6">
+        <v>17</v>
+      </c>
     </row>
     <row r="51" spans="1:10" ht="42.75" thickBot="1">
       <c r="A51" s="7"/>
@@ -5204,19 +5437,17 @@
     <mergeCell ref="H26:H36"/>
     <mergeCell ref="I26:I36"/>
     <mergeCell ref="J2:J12"/>
+    <mergeCell ref="A2:A12"/>
     <mergeCell ref="A75:A85"/>
     <mergeCell ref="B75:B85"/>
     <mergeCell ref="C75:C85"/>
     <mergeCell ref="H75:H85"/>
     <mergeCell ref="I75:I85"/>
-    <mergeCell ref="J75:J85"/>
-    <mergeCell ref="A38:A48"/>
     <mergeCell ref="B38:B48"/>
     <mergeCell ref="C38:C48"/>
     <mergeCell ref="H38:H48"/>
     <mergeCell ref="I38:I48"/>
     <mergeCell ref="J38:J48"/>
-    <mergeCell ref="A2:A12"/>
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="C2:C12"/>
     <mergeCell ref="J87:J97"/>
@@ -5231,6 +5462,8 @@
     <mergeCell ref="C87:C97"/>
     <mergeCell ref="H87:H97"/>
     <mergeCell ref="I87:I97"/>
+    <mergeCell ref="J75:J85"/>
+    <mergeCell ref="A38:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5259,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5329,7 +5562,9 @@
       <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6"/>
+      <c r="J2" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="42.75" thickBot="1">
       <c r="A3" s="7"/>
@@ -5477,7 +5712,9 @@
       <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="6"/>
+      <c r="J10" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="42.75" thickBot="1">
       <c r="A11" s="7"/>
@@ -5625,7 +5862,9 @@
       <c r="I18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="42.75" thickBot="1">
       <c r="A19" s="7"/>
@@ -5773,7 +6012,9 @@
       <c r="I26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="6"/>
+      <c r="J26" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="42.75" thickBot="1">
       <c r="A27" s="7"/>
@@ -6118,8 +6359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7300,11 +7541,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A57:A65"/>
-    <mergeCell ref="B57:B65"/>
-    <mergeCell ref="C57:C65"/>
-    <mergeCell ref="H57:H65"/>
-    <mergeCell ref="I57:I65"/>
     <mergeCell ref="J57:J65"/>
     <mergeCell ref="A46:A55"/>
     <mergeCell ref="B46:B55"/>
@@ -7312,11 +7548,11 @@
     <mergeCell ref="H46:H55"/>
     <mergeCell ref="I46:I55"/>
     <mergeCell ref="J46:J55"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="B35:B44"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="H35:H44"/>
-    <mergeCell ref="I35:I44"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="B57:B65"/>
+    <mergeCell ref="C57:C65"/>
+    <mergeCell ref="H57:H65"/>
+    <mergeCell ref="I57:I65"/>
     <mergeCell ref="J35:J44"/>
     <mergeCell ref="A24:A33"/>
     <mergeCell ref="B24:B33"/>
@@ -7324,11 +7560,11 @@
     <mergeCell ref="H24:H33"/>
     <mergeCell ref="I24:I33"/>
     <mergeCell ref="J24:J33"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="B13:B22"/>
-    <mergeCell ref="C13:C22"/>
-    <mergeCell ref="H13:H22"/>
-    <mergeCell ref="I13:I22"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="B35:B44"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="H35:H44"/>
+    <mergeCell ref="I35:I44"/>
     <mergeCell ref="J13:J22"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B2:B11"/>
@@ -7336,6 +7572,11 @@
     <mergeCell ref="H2:H11"/>
     <mergeCell ref="I2:I11"/>
     <mergeCell ref="J2:J11"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="C13:C22"/>
+    <mergeCell ref="H13:H22"/>
+    <mergeCell ref="I13:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -7363,8 +7604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:C38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8243,11 +8485,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B40:B46"/>
-    <mergeCell ref="C40:C46"/>
-    <mergeCell ref="H40:H46"/>
-    <mergeCell ref="I40:I46"/>
     <mergeCell ref="J40:J46"/>
     <mergeCell ref="A31:A38"/>
     <mergeCell ref="B31:B38"/>
@@ -8255,11 +8492,11 @@
     <mergeCell ref="H31:H38"/>
     <mergeCell ref="I31:I38"/>
     <mergeCell ref="J31:J38"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="B22:B29"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="H22:H29"/>
-    <mergeCell ref="I22:I29"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="C40:C46"/>
+    <mergeCell ref="H40:H46"/>
+    <mergeCell ref="I40:I46"/>
     <mergeCell ref="J22:J29"/>
     <mergeCell ref="A12:A20"/>
     <mergeCell ref="B12:B20"/>
@@ -8267,12 +8504,17 @@
     <mergeCell ref="H12:H20"/>
     <mergeCell ref="I12:I20"/>
     <mergeCell ref="J12:J20"/>
+    <mergeCell ref="A22:A29"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="H22:H29"/>
+    <mergeCell ref="I22:I29"/>
+    <mergeCell ref="J2:J10"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="H2:H10"/>
     <mergeCell ref="I2:I10"/>
-    <mergeCell ref="J2:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>